<commit_message>
Um pouco de organização
</commit_message>
<xml_diff>
--- a/doc/editor.xlsx
+++ b/doc/editor.xlsx
@@ -65,9 +65,6 @@
     <t>Guarda o id de cada página (usada para os links)</t>
   </si>
   <si>
-    <t>\{([:pagina:]( [:pagina:])*)?\}</t>
-  </si>
-  <si>
     <t>Objeto de texto</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>[1-9][0-9]*</t>
   </si>
   <si>
-    <t>GROB [1-9][0-9]* [1-9][0-9]* [0-9A-F]+</t>
-  </si>
-  <si>
     <t>Folha do índice</t>
   </si>
   <si>
@@ -122,21 +116,12 @@
     <t>Define como o objeto deve estar alinhado na página (-1 = esquerda, 0 = centralizado, 1 = direita)</t>
   </si>
   <si>
-    <t>\{[:alinhamento:] [:string:] 1\}</t>
-  </si>
-  <si>
     <t>Objeto de régua</t>
   </si>
   <si>
     <t>Representa um linha horizontal</t>
   </si>
   <si>
-    <t>\{[:string:] [:id:] 1\}</t>
-  </si>
-  <si>
-    <t>\{([:objeto:]( [:objeto:])*)?\}</t>
-  </si>
-  <si>
     <t>[:objTexto:]|[:objEquacao:]|[:objImagem:]|[:objCabecalho:]|[:objRegua:]</t>
   </si>
   <si>
@@ -152,39 +137,15 @@
     <t>Representa um anexo</t>
   </si>
   <si>
-    <t>\{[:string:] [:string:]\}</t>
-  </si>
-  <si>
-    <t>\{([:anexo:]( [:anexo:])*)?\}</t>
-  </si>
-  <si>
-    <t>\{[:alinhamento:] [:nivel:] [:string:] 3\}</t>
-  </si>
-  <si>
     <t>Sub índice</t>
   </si>
   <si>
     <t>Indica um índice com filhos</t>
   </si>
   <si>
-    <t>\{[:string:]( [:subIndice:]| [:folhaIndice:])* 0\}</t>
-  </si>
-  <si>
-    <t>\{([:subIndice:]|[:folhaIndice:]( [:subIndice:]| [:folhaIndice:])*)?\}</t>
-  </si>
-  <si>
     <t>Strings</t>
   </si>
   <si>
-    <t>\{([:string:]( [:string:])*)?\}</t>
-  </si>
-  <si>
-    <t>"[^"]*"</t>
-  </si>
-  <si>
-    <t>\{[1-9] [:string:] [:edicao:] [:indice:] [:paginas:] [:anexos:] [:strings:]\}</t>
-  </si>
-  <si>
     <t>Opções de edição</t>
   </si>
   <si>
@@ -194,22 +155,61 @@
     <t>Dados lidos somente pelo editor: data de criação, data de modificação, auto paginação, auto indexação</t>
   </si>
   <si>
-    <t>\{[0-9]+ [0-9]+ [01] [01]\}</t>
-  </si>
-  <si>
     <t>Representa um objeto de texto simples (cada string é colocada numa linha)</t>
   </si>
   <si>
-    <t>\{[:imagem:] 2\}</t>
-  </si>
-  <si>
-    <t>\{[:alinhamento:] [:strings:] 0\}</t>
-  </si>
-  <si>
     <t>Guarda a representação string de cada página (usada para fazer buscas) ou o texto de cada linha</t>
   </si>
   <si>
-    <t>\{[:altura:] 4\}</t>
+    <t>{[1-9] [:string:] [:edicao:] [:indice:] [:paginas:] [:anexos:] [:strings:]}</t>
+  </si>
+  <si>
+    <t>{[0-9]+ [0-9]+ [01] [01]}</t>
+  </si>
+  <si>
+    <t>{([:subIndice:]|[:folhaIndice:])*}</t>
+  </si>
+  <si>
+    <t>{[:string:] ([:subIndice:]|[:folhaIndice:])* 0}</t>
+  </si>
+  <si>
+    <t>{[:string:] [:id:] 1}</t>
+  </si>
+  <si>
+    <t>{[:pagina:]*}</t>
+  </si>
+  <si>
+    <t>{[:anexo:]*}</t>
+  </si>
+  <si>
+    <t>{[:objeto:]*}</t>
+  </si>
+  <si>
+    <t>{[:string:] [:string:]}</t>
+  </si>
+  <si>
+    <t>{[:string:]*}</t>
+  </si>
+  <si>
+    <t>{[:alinhamento:] [:strings:] 0}</t>
+  </si>
+  <si>
+    <t>{[:alinhamento:] [:string:] 1}</t>
+  </si>
+  <si>
+    <t>{[:imagem:] 2}</t>
+  </si>
+  <si>
+    <t>{[:alinhamento:] [:nivel:] [:string:] 3}</t>
+  </si>
+  <si>
+    <t>{[:altura:] 4}</t>
+  </si>
+  <si>
+    <t>GROB [0-9]+ [0-9]+ [0-9A-F]+</t>
+  </si>
+  <si>
+    <t>".*"</t>
   </si>
 </sst>
 </file>
@@ -717,7 +717,7 @@
     <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="C3" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -763,10 +763,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -784,13 +784,13 @@
     <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="C11" s="5" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -814,7 +814,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -829,16 +829,16 @@
       <c r="K14" s="8"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="C15" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -856,13 +856,13 @@
     <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="C17" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -886,7 +886,7 @@
         <v>12</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="G19" s="1"/>
     </row>
@@ -910,7 +910,7 @@
         <v>13</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -928,13 +928,13 @@
     <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="C23" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -952,13 +952,13 @@
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="C25" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -976,13 +976,13 @@
     <row r="27" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="C27" s="5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G27" s="1"/>
     </row>
@@ -1006,7 +1006,7 @@
         <v>15</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -1030,7 +1030,7 @@
         <v>6</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -1048,13 +1048,13 @@
     <row r="33" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="C33" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -1072,13 +1072,13 @@
     <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="C35" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="G35" s="1"/>
     </row>
@@ -1096,13 +1096,13 @@
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="C37" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G37" s="1"/>
     </row>
@@ -1120,13 +1120,13 @@
     <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="C39" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -1144,13 +1144,13 @@
     <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="C41" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G41" s="1"/>
     </row>
@@ -1168,13 +1168,13 @@
     <row r="43" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="C43" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E43" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="G43" s="1"/>
     </row>
@@ -1192,13 +1192,13 @@
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="C45" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="G45" s="1"/>
     </row>
@@ -1219,10 +1219,10 @@
         <v>4</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="G47" s="1"/>
     </row>

</xml_diff>